<commit_message>
some work from garrett I think
</commit_message>
<xml_diff>
--- a/python/exports/Export.xlsx
+++ b/python/exports/Export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K307"/>
+  <dimension ref="A1:K289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12890,996 +12890,6 @@
       </c>
       <c r="K289" t="inlineStr"/>
     </row>
-    <row r="290">
-      <c r="A290" t="n">
-        <v>0</v>
-      </c>
-      <c r="B290" t="inlineStr">
-        <is>
-          <t>Add</t>
-        </is>
-      </c>
-      <c r="C290" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D290" t="inlineStr">
-        <is>
-          <t>here@example.net</t>
-        </is>
-      </c>
-      <c r="E290" t="inlineStr">
-        <is>
-          <t>22333</t>
-        </is>
-      </c>
-      <c r="F290" t="inlineStr">
-        <is>
-          <t>Town</t>
-        </is>
-      </c>
-      <c r="G290" t="inlineStr">
-        <is>
-          <t>SK</t>
-        </is>
-      </c>
-      <c r="H290" t="inlineStr">
-        <is>
-          <t>233 Highway Blvd</t>
-        </is>
-      </c>
-      <c r="I290" t="inlineStr">
-        <is>
-          <t>1235831294.0</t>
-        </is>
-      </c>
-      <c r="J290" t="inlineStr">
-        <is>
-          <t>Genderqueer</t>
-        </is>
-      </c>
-      <c r="K290" t="inlineStr">
-        <is>
-          <t>Added the example!</t>
-        </is>
-      </c>
-    </row>
-    <row r="291">
-      <c r="A291" t="n">
-        <v>0</v>
-      </c>
-      <c r="B291" t="inlineStr">
-        <is>
-          <t>Flamebreaker</t>
-        </is>
-      </c>
-      <c r="C291" t="inlineStr">
-        <is>
-          <t>Feljer</t>
-        </is>
-      </c>
-      <c r="D291" t="inlineStr">
-        <is>
-          <t>flame@frozensky.gov</t>
-        </is>
-      </c>
-      <c r="E291" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F291" t="inlineStr">
-        <is>
-          <t>Frozen Sky Village</t>
-        </is>
-      </c>
-      <c r="G291" t="inlineStr">
-        <is>
-          <t>NU</t>
-        </is>
-      </c>
-      <c r="H291" t="inlineStr">
-        <is>
-          <t>1 Crystal Wing Palace</t>
-        </is>
-      </c>
-      <c r="I291" t="inlineStr">
-        <is>
-          <t>19684620572.0</t>
-        </is>
-      </c>
-      <c r="J291" t="inlineStr">
-        <is>
-          <t>Bigender</t>
-        </is>
-      </c>
-      <c r="K291" t="inlineStr">
-        <is>
-          <t>Needs more gilded dragons</t>
-        </is>
-      </c>
-    </row>
-    <row r="292">
-      <c r="A292" t="n">
-        <v>0</v>
-      </c>
-      <c r="B292" t="inlineStr">
-        <is>
-          <t>Add</t>
-        </is>
-      </c>
-      <c r="C292" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D292" t="inlineStr">
-        <is>
-          <t>here@example.net</t>
-        </is>
-      </c>
-      <c r="E292" t="inlineStr">
-        <is>
-          <t>22333</t>
-        </is>
-      </c>
-      <c r="F292" t="inlineStr">
-        <is>
-          <t>Town</t>
-        </is>
-      </c>
-      <c r="G292" t="inlineStr">
-        <is>
-          <t>SK</t>
-        </is>
-      </c>
-      <c r="H292" t="inlineStr">
-        <is>
-          <t>233 Highway Blvd</t>
-        </is>
-      </c>
-      <c r="I292" t="inlineStr">
-        <is>
-          <t>1235831294.0</t>
-        </is>
-      </c>
-      <c r="J292" t="inlineStr">
-        <is>
-          <t>Genderqueer</t>
-        </is>
-      </c>
-      <c r="K292" t="inlineStr">
-        <is>
-          <t>Added the example!</t>
-        </is>
-      </c>
-    </row>
-    <row r="293">
-      <c r="A293" t="n">
-        <v>0</v>
-      </c>
-      <c r="B293" t="inlineStr">
-        <is>
-          <t>Flamebreaker</t>
-        </is>
-      </c>
-      <c r="C293" t="inlineStr">
-        <is>
-          <t>Feljer</t>
-        </is>
-      </c>
-      <c r="D293" t="inlineStr">
-        <is>
-          <t>flame@frozensky.gov</t>
-        </is>
-      </c>
-      <c r="E293" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F293" t="inlineStr">
-        <is>
-          <t>Frozen Sky Village</t>
-        </is>
-      </c>
-      <c r="G293" t="inlineStr">
-        <is>
-          <t>NU</t>
-        </is>
-      </c>
-      <c r="H293" t="inlineStr">
-        <is>
-          <t>1 Crystal Wing Palace</t>
-        </is>
-      </c>
-      <c r="I293" t="inlineStr">
-        <is>
-          <t>19684620572.0</t>
-        </is>
-      </c>
-      <c r="J293" t="inlineStr">
-        <is>
-          <t>Bigender</t>
-        </is>
-      </c>
-      <c r="K293" t="inlineStr">
-        <is>
-          <t>Needs more gilded dragons</t>
-        </is>
-      </c>
-    </row>
-    <row r="294">
-      <c r="A294" t="n">
-        <v>0</v>
-      </c>
-      <c r="B294" t="inlineStr">
-        <is>
-          <t>Add</t>
-        </is>
-      </c>
-      <c r="C294" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D294" t="inlineStr">
-        <is>
-          <t>here@example.net</t>
-        </is>
-      </c>
-      <c r="E294" t="inlineStr">
-        <is>
-          <t>22333</t>
-        </is>
-      </c>
-      <c r="F294" t="inlineStr">
-        <is>
-          <t>Town</t>
-        </is>
-      </c>
-      <c r="G294" t="inlineStr">
-        <is>
-          <t>SK</t>
-        </is>
-      </c>
-      <c r="H294" t="inlineStr">
-        <is>
-          <t>233 Highway Blvd</t>
-        </is>
-      </c>
-      <c r="I294" t="inlineStr">
-        <is>
-          <t>1235831294.0</t>
-        </is>
-      </c>
-      <c r="J294" t="inlineStr">
-        <is>
-          <t>Genderqueer</t>
-        </is>
-      </c>
-      <c r="K294" t="inlineStr">
-        <is>
-          <t>Added the example!</t>
-        </is>
-      </c>
-    </row>
-    <row r="295">
-      <c r="A295" t="n">
-        <v>0</v>
-      </c>
-      <c r="B295" t="inlineStr">
-        <is>
-          <t>Flamebreaker</t>
-        </is>
-      </c>
-      <c r="C295" t="inlineStr">
-        <is>
-          <t>Feljer</t>
-        </is>
-      </c>
-      <c r="D295" t="inlineStr">
-        <is>
-          <t>flame@frozensky.gov</t>
-        </is>
-      </c>
-      <c r="E295" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F295" t="inlineStr">
-        <is>
-          <t>Frozen Sky Village</t>
-        </is>
-      </c>
-      <c r="G295" t="inlineStr">
-        <is>
-          <t>NU</t>
-        </is>
-      </c>
-      <c r="H295" t="inlineStr">
-        <is>
-          <t>1 Crystal Wing Palace</t>
-        </is>
-      </c>
-      <c r="I295" t="inlineStr">
-        <is>
-          <t>19684620572.0</t>
-        </is>
-      </c>
-      <c r="J295" t="inlineStr">
-        <is>
-          <t>Bigender</t>
-        </is>
-      </c>
-      <c r="K295" t="inlineStr">
-        <is>
-          <t>Needs more gilded dragons</t>
-        </is>
-      </c>
-    </row>
-    <row r="296">
-      <c r="A296" t="n">
-        <v>0</v>
-      </c>
-      <c r="B296" t="inlineStr">
-        <is>
-          <t>Add</t>
-        </is>
-      </c>
-      <c r="C296" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D296" t="inlineStr">
-        <is>
-          <t>here@example.net</t>
-        </is>
-      </c>
-      <c r="E296" t="inlineStr">
-        <is>
-          <t>22333</t>
-        </is>
-      </c>
-      <c r="F296" t="inlineStr">
-        <is>
-          <t>Town</t>
-        </is>
-      </c>
-      <c r="G296" t="inlineStr">
-        <is>
-          <t>SK</t>
-        </is>
-      </c>
-      <c r="H296" t="inlineStr">
-        <is>
-          <t>233 Highway Blvd</t>
-        </is>
-      </c>
-      <c r="I296" t="inlineStr">
-        <is>
-          <t>1235831294.0</t>
-        </is>
-      </c>
-      <c r="J296" t="inlineStr">
-        <is>
-          <t>Genderqueer</t>
-        </is>
-      </c>
-      <c r="K296" t="inlineStr">
-        <is>
-          <t>Added the example!</t>
-        </is>
-      </c>
-    </row>
-    <row r="297">
-      <c r="A297" t="n">
-        <v>0</v>
-      </c>
-      <c r="B297" t="inlineStr">
-        <is>
-          <t>Flamebreaker</t>
-        </is>
-      </c>
-      <c r="C297" t="inlineStr">
-        <is>
-          <t>Feljer</t>
-        </is>
-      </c>
-      <c r="D297" t="inlineStr">
-        <is>
-          <t>flame@frozensky.gov</t>
-        </is>
-      </c>
-      <c r="E297" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F297" t="inlineStr">
-        <is>
-          <t>Frozen Sky Village</t>
-        </is>
-      </c>
-      <c r="G297" t="inlineStr">
-        <is>
-          <t>NU</t>
-        </is>
-      </c>
-      <c r="H297" t="inlineStr">
-        <is>
-          <t>1 Crystal Wing Palace</t>
-        </is>
-      </c>
-      <c r="I297" t="inlineStr">
-        <is>
-          <t>19684620572.0</t>
-        </is>
-      </c>
-      <c r="J297" t="inlineStr">
-        <is>
-          <t>Bigender</t>
-        </is>
-      </c>
-      <c r="K297" t="inlineStr">
-        <is>
-          <t>Needs more gilded dragons</t>
-        </is>
-      </c>
-    </row>
-    <row r="298">
-      <c r="A298" t="n">
-        <v>0</v>
-      </c>
-      <c r="B298" t="inlineStr">
-        <is>
-          <t>Add</t>
-        </is>
-      </c>
-      <c r="C298" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D298" t="inlineStr">
-        <is>
-          <t>here@example.net</t>
-        </is>
-      </c>
-      <c r="E298" t="inlineStr">
-        <is>
-          <t>22333</t>
-        </is>
-      </c>
-      <c r="F298" t="inlineStr">
-        <is>
-          <t>Town</t>
-        </is>
-      </c>
-      <c r="G298" t="inlineStr">
-        <is>
-          <t>SK</t>
-        </is>
-      </c>
-      <c r="H298" t="inlineStr">
-        <is>
-          <t>233 Highway Blvd</t>
-        </is>
-      </c>
-      <c r="I298" t="inlineStr">
-        <is>
-          <t>1235831294.0</t>
-        </is>
-      </c>
-      <c r="J298" t="inlineStr">
-        <is>
-          <t>Genderqueer</t>
-        </is>
-      </c>
-      <c r="K298" t="inlineStr">
-        <is>
-          <t>Added the example!</t>
-        </is>
-      </c>
-    </row>
-    <row r="299">
-      <c r="A299" t="n">
-        <v>0</v>
-      </c>
-      <c r="B299" t="inlineStr">
-        <is>
-          <t>Flamebreaker</t>
-        </is>
-      </c>
-      <c r="C299" t="inlineStr">
-        <is>
-          <t>Feljer</t>
-        </is>
-      </c>
-      <c r="D299" t="inlineStr">
-        <is>
-          <t>flame@frozensky.gov</t>
-        </is>
-      </c>
-      <c r="E299" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F299" t="inlineStr">
-        <is>
-          <t>Frozen Sky Village</t>
-        </is>
-      </c>
-      <c r="G299" t="inlineStr">
-        <is>
-          <t>NU</t>
-        </is>
-      </c>
-      <c r="H299" t="inlineStr">
-        <is>
-          <t>1 Crystal Wing Palace</t>
-        </is>
-      </c>
-      <c r="I299" t="inlineStr">
-        <is>
-          <t>19684620572.0</t>
-        </is>
-      </c>
-      <c r="J299" t="inlineStr">
-        <is>
-          <t>Bigender</t>
-        </is>
-      </c>
-      <c r="K299" t="inlineStr">
-        <is>
-          <t>Needs more gilded dragons</t>
-        </is>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300" t="n">
-        <v>0</v>
-      </c>
-      <c r="B300" t="inlineStr">
-        <is>
-          <t>Add</t>
-        </is>
-      </c>
-      <c r="C300" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D300" t="inlineStr">
-        <is>
-          <t>here@example.net</t>
-        </is>
-      </c>
-      <c r="E300" t="inlineStr">
-        <is>
-          <t>22333</t>
-        </is>
-      </c>
-      <c r="F300" t="inlineStr">
-        <is>
-          <t>Town</t>
-        </is>
-      </c>
-      <c r="G300" t="inlineStr">
-        <is>
-          <t>SK</t>
-        </is>
-      </c>
-      <c r="H300" t="inlineStr">
-        <is>
-          <t>233 Highway Blvd</t>
-        </is>
-      </c>
-      <c r="I300" t="inlineStr">
-        <is>
-          <t>1235831294.0</t>
-        </is>
-      </c>
-      <c r="J300" t="inlineStr">
-        <is>
-          <t>Genderqueer</t>
-        </is>
-      </c>
-      <c r="K300" t="inlineStr">
-        <is>
-          <t>Added the example!</t>
-        </is>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301" t="n">
-        <v>0</v>
-      </c>
-      <c r="B301" t="inlineStr">
-        <is>
-          <t>Flamebreaker</t>
-        </is>
-      </c>
-      <c r="C301" t="inlineStr">
-        <is>
-          <t>Feljer</t>
-        </is>
-      </c>
-      <c r="D301" t="inlineStr">
-        <is>
-          <t>flame@frozensky.gov</t>
-        </is>
-      </c>
-      <c r="E301" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F301" t="inlineStr">
-        <is>
-          <t>Frozen Sky Village</t>
-        </is>
-      </c>
-      <c r="G301" t="inlineStr">
-        <is>
-          <t>NU</t>
-        </is>
-      </c>
-      <c r="H301" t="inlineStr">
-        <is>
-          <t>1 Crystal Wing Palace</t>
-        </is>
-      </c>
-      <c r="I301" t="inlineStr">
-        <is>
-          <t>19684620572.0</t>
-        </is>
-      </c>
-      <c r="J301" t="inlineStr">
-        <is>
-          <t>Bigender</t>
-        </is>
-      </c>
-      <c r="K301" t="inlineStr">
-        <is>
-          <t>Needs more gilded dragons</t>
-        </is>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" t="n">
-        <v>0</v>
-      </c>
-      <c r="B302" t="inlineStr">
-        <is>
-          <t>Add</t>
-        </is>
-      </c>
-      <c r="C302" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D302" t="inlineStr">
-        <is>
-          <t>here@example.net</t>
-        </is>
-      </c>
-      <c r="E302" t="inlineStr">
-        <is>
-          <t>22333</t>
-        </is>
-      </c>
-      <c r="F302" t="inlineStr">
-        <is>
-          <t>Town</t>
-        </is>
-      </c>
-      <c r="G302" t="inlineStr">
-        <is>
-          <t>SK</t>
-        </is>
-      </c>
-      <c r="H302" t="inlineStr">
-        <is>
-          <t>233 Highway Blvd</t>
-        </is>
-      </c>
-      <c r="I302" t="inlineStr">
-        <is>
-          <t>1235831294.0</t>
-        </is>
-      </c>
-      <c r="J302" t="inlineStr">
-        <is>
-          <t>Genderqueer</t>
-        </is>
-      </c>
-      <c r="K302" t="inlineStr">
-        <is>
-          <t>Added the example!</t>
-        </is>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" t="n">
-        <v>0</v>
-      </c>
-      <c r="B303" t="inlineStr">
-        <is>
-          <t>Flamebreaker</t>
-        </is>
-      </c>
-      <c r="C303" t="inlineStr">
-        <is>
-          <t>Feljer</t>
-        </is>
-      </c>
-      <c r="D303" t="inlineStr">
-        <is>
-          <t>flame@frozensky.gov</t>
-        </is>
-      </c>
-      <c r="E303" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F303" t="inlineStr">
-        <is>
-          <t>Frozen Sky Village</t>
-        </is>
-      </c>
-      <c r="G303" t="inlineStr">
-        <is>
-          <t>NU</t>
-        </is>
-      </c>
-      <c r="H303" t="inlineStr">
-        <is>
-          <t>1 Crystal Wing Palace</t>
-        </is>
-      </c>
-      <c r="I303" t="inlineStr">
-        <is>
-          <t>19684620572.0</t>
-        </is>
-      </c>
-      <c r="J303" t="inlineStr">
-        <is>
-          <t>Bigender</t>
-        </is>
-      </c>
-      <c r="K303" t="inlineStr">
-        <is>
-          <t>Needs more gilded dragons</t>
-        </is>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304" t="n">
-        <v>0</v>
-      </c>
-      <c r="B304" t="inlineStr">
-        <is>
-          <t>Add</t>
-        </is>
-      </c>
-      <c r="C304" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D304" t="inlineStr">
-        <is>
-          <t>here@example.net</t>
-        </is>
-      </c>
-      <c r="E304" t="inlineStr">
-        <is>
-          <t>22333</t>
-        </is>
-      </c>
-      <c r="F304" t="inlineStr">
-        <is>
-          <t>Town</t>
-        </is>
-      </c>
-      <c r="G304" t="inlineStr">
-        <is>
-          <t>SK</t>
-        </is>
-      </c>
-      <c r="H304" t="inlineStr">
-        <is>
-          <t>233 Highway Blvd</t>
-        </is>
-      </c>
-      <c r="I304" t="inlineStr">
-        <is>
-          <t>1235831294.0</t>
-        </is>
-      </c>
-      <c r="J304" t="inlineStr">
-        <is>
-          <t>Genderqueer</t>
-        </is>
-      </c>
-      <c r="K304" t="inlineStr">
-        <is>
-          <t>Added the example!</t>
-        </is>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305" t="n">
-        <v>0</v>
-      </c>
-      <c r="B305" t="inlineStr">
-        <is>
-          <t>Flamebreaker</t>
-        </is>
-      </c>
-      <c r="C305" t="inlineStr">
-        <is>
-          <t>Feljer</t>
-        </is>
-      </c>
-      <c r="D305" t="inlineStr">
-        <is>
-          <t>flame@frozensky.gov</t>
-        </is>
-      </c>
-      <c r="E305" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F305" t="inlineStr">
-        <is>
-          <t>Frozen Sky Village</t>
-        </is>
-      </c>
-      <c r="G305" t="inlineStr">
-        <is>
-          <t>NU</t>
-        </is>
-      </c>
-      <c r="H305" t="inlineStr">
-        <is>
-          <t>1 Crystal Wing Palace</t>
-        </is>
-      </c>
-      <c r="I305" t="inlineStr">
-        <is>
-          <t>19684620572.0</t>
-        </is>
-      </c>
-      <c r="J305" t="inlineStr">
-        <is>
-          <t>Bigender</t>
-        </is>
-      </c>
-      <c r="K305" t="inlineStr">
-        <is>
-          <t>Needs more gilded dragons</t>
-        </is>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" t="n">
-        <v>0</v>
-      </c>
-      <c r="B306" t="inlineStr">
-        <is>
-          <t>Add</t>
-        </is>
-      </c>
-      <c r="C306" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D306" t="inlineStr">
-        <is>
-          <t>here@example.net</t>
-        </is>
-      </c>
-      <c r="E306" t="inlineStr">
-        <is>
-          <t>22333</t>
-        </is>
-      </c>
-      <c r="F306" t="inlineStr">
-        <is>
-          <t>Town</t>
-        </is>
-      </c>
-      <c r="G306" t="inlineStr">
-        <is>
-          <t>SK</t>
-        </is>
-      </c>
-      <c r="H306" t="inlineStr">
-        <is>
-          <t>233 Highway Blvd</t>
-        </is>
-      </c>
-      <c r="I306" t="inlineStr">
-        <is>
-          <t>1235831294.0</t>
-        </is>
-      </c>
-      <c r="J306" t="inlineStr">
-        <is>
-          <t>Genderqueer</t>
-        </is>
-      </c>
-      <c r="K306" t="inlineStr">
-        <is>
-          <t>Added the example!</t>
-        </is>
-      </c>
-    </row>
-    <row r="307">
-      <c r="A307" t="n">
-        <v>0</v>
-      </c>
-      <c r="B307" t="inlineStr">
-        <is>
-          <t>Flamebreaker</t>
-        </is>
-      </c>
-      <c r="C307" t="inlineStr">
-        <is>
-          <t>Feljer</t>
-        </is>
-      </c>
-      <c r="D307" t="inlineStr">
-        <is>
-          <t>flame@frozensky.gov</t>
-        </is>
-      </c>
-      <c r="E307" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F307" t="inlineStr">
-        <is>
-          <t>Frozen Sky Village</t>
-        </is>
-      </c>
-      <c r="G307" t="inlineStr">
-        <is>
-          <t>NU</t>
-        </is>
-      </c>
-      <c r="H307" t="inlineStr">
-        <is>
-          <t>1 Crystal Wing Palace</t>
-        </is>
-      </c>
-      <c r="I307" t="inlineStr">
-        <is>
-          <t>19684620572.0</t>
-        </is>
-      </c>
-      <c r="J307" t="inlineStr">
-        <is>
-          <t>Bigender</t>
-        </is>
-      </c>
-      <c r="K307" t="inlineStr">
-        <is>
-          <t>Needs more gilded dragons</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>